<commit_message>
Changes to spreadsheet, added tests for walkways
</commit_message>
<xml_diff>
--- a/ourClueLayout.xlsx
+++ b/ourClueLayout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="7425"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20835" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="54">
   <si>
     <t>Table 1</t>
   </si>
@@ -143,17 +143,47 @@
     <t>Room Initials tests</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of Doors: </t>
-  </si>
-  <si>
     <t>Number of Doors: 18</t>
+  </si>
+  <si>
+    <t>walkway Cell tests</t>
+  </si>
+  <si>
+    <t>Adjacency edge tests</t>
+  </si>
+  <si>
+    <t>Adjacency next to room</t>
+  </si>
+  <si>
+    <t>Adjacency next to doorway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walkway Adjacent </t>
+  </si>
+  <si>
+    <t>Near door wrong direction</t>
+  </si>
+  <si>
+    <t>Inside doors</t>
+  </si>
+  <si>
+    <t>Walkway Cell target Tests (4)</t>
+  </si>
+  <si>
+    <t>Enter room target tests (2)</t>
+  </si>
+  <si>
+    <t>Enter room shortcut (2)</t>
+  </si>
+  <si>
+    <t>Exit room target tests (2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -178,8 +208,13 @@
       <sz val="10"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +263,72 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA90F8C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDA9916"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF990099"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -258,7 +359,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -305,6 +406,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -381,6 +533,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF990099"/>
+      <color rgb="FFFF6699"/>
+      <color rgb="FF666699"/>
+      <color rgb="FFFF66FF"/>
+      <color rgb="FFDA9916"/>
+      <color rgb="FF000000"/>
+      <color rgb="FF009999"/>
+      <color rgb="FFA90F8C"/>
       <color rgb="FFCCCC00"/>
     </mruColors>
   </colors>
@@ -1639,15 +1799,17 @@
   </sheetPr>
   <dimension ref="A1:IV32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC9" sqref="AC9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="26" width="3" style="1" customWidth="1"/>
-    <col min="27" max="27" width="12.796875" style="1" customWidth="1"/>
-    <col min="28" max="256" width="9.09765625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="18.19921875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="9.09765625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="13.296875" style="1" customWidth="1"/>
+    <col min="30" max="256" width="9.09765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="15" x14ac:dyDescent="0.2">
@@ -1739,7 +1901,7 @@
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1769,7 +1931,7 @@
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="22" t="s">
         <v>2</v>
       </c>
       <c r="Q2" s="4" t="s">
@@ -1784,7 +1946,7 @@
       <c r="T2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="31" t="s">
         <v>2</v>
       </c>
       <c r="V2" s="5">
@@ -1973,7 +2135,7 @@
       <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="31" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -2111,7 +2273,7 @@
       <c r="L5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="27" t="s">
         <v>11</v>
       </c>
       <c r="N5" s="2" t="s">
@@ -2135,7 +2297,7 @@
       <c r="T5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="U5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="V5" s="5">
@@ -2149,7 +2311,9 @@
         <v>40</v>
       </c>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
+      <c r="AC5" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="AD5" s="6"/>
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
@@ -2225,10 +2389,10 @@
       <c r="K6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="L6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -2378,8 +2542,8 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6" t="s">
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AB7" s="6"/>
@@ -2432,7 +2596,7 @@
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2450,7 +2614,7 @@
       <c r="H8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="29" t="s">
         <v>2</v>
       </c>
       <c r="J8" s="3" t="s">
@@ -2477,7 +2641,7 @@
       <c r="Q8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="20" t="s">
         <v>2</v>
       </c>
       <c r="S8" s="3" t="s">
@@ -2486,7 +2650,7 @@
       <c r="T8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="U8" s="18" t="s">
         <v>2</v>
       </c>
       <c r="V8" s="5">
@@ -2495,8 +2659,10 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
       <c r="AD8" s="6"/>
@@ -2610,8 +2776,10 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
       <c r="AD9" s="6"/>
@@ -2674,7 +2842,7 @@
       <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="30" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -2725,9 +2893,9 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
+      <c r="Z10" s="21"/>
       <c r="AA10" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
@@ -2842,8 +3010,10 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
@@ -2906,7 +3076,7 @@
       <c r="F12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="22" t="s">
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
@@ -2936,7 +3106,7 @@
       <c r="P12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="Q12" s="27" t="s">
         <v>16</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -2957,12 +3127,14 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
+      <c r="Z12" s="25"/>
       <c r="AA12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
@@ -3074,14 +3246,16 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
-      <c r="Z13" s="5" t="s">
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="AC13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
@@ -3193,14 +3367,16 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
-      <c r="Z14" s="5" t="s">
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AA14" s="5" t="s">
+      <c r="AC14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
       <c r="AD14" s="6"/>
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
@@ -3300,7 +3476,7 @@
       <c r="S15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T15" s="3" t="s">
+      <c r="T15" s="16" t="s">
         <v>2</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -3312,14 +3488,16 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
-      <c r="Z15" s="5" t="s">
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AA15" s="5" t="s">
+      <c r="AC15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
       <c r="AF15" s="6"/>
@@ -3410,7 +3588,7 @@
       <c r="P16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="Q16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="R16" s="2" t="s">
@@ -3431,14 +3609,16 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
-      <c r="Z16" s="5" t="s">
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AA16" s="5" t="s">
+      <c r="AC16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="6"/>
       <c r="AF16" s="6"/>
@@ -3487,7 +3667,7 @@
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -3505,7 +3685,7 @@
       <c r="H17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="24" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="3" t="s">
@@ -3550,14 +3730,16 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
-      <c r="Z17" s="5" t="s">
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AC17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
       <c r="AF17" s="6"/>
@@ -3600,7 +3782,7 @@
       <c r="BQ17" s="6"/>
     </row>
     <row r="18" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -3669,14 +3851,14 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
-      <c r="Z18" s="5" t="s">
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AA18" s="5" t="s">
+      <c r="AC18" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
       <c r="AF18" s="6"/>
@@ -3737,7 +3919,7 @@
       <c r="F19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="32" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="3" t="s">
@@ -3770,7 +3952,7 @@
       <c r="Q19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R19" s="3" t="s">
+      <c r="R19" s="22" t="s">
         <v>2</v>
       </c>
       <c r="S19" s="3" t="s">
@@ -3779,7 +3961,7 @@
       <c r="T19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="U19" s="3" t="s">
+      <c r="U19" s="29" t="s">
         <v>2</v>
       </c>
       <c r="V19" s="5">
@@ -3788,14 +3970,14 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
-      <c r="Z19" s="5" t="s">
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="5"/>
+      <c r="AB19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AA19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="6"/>
       <c r="AF19" s="6"/>
@@ -3907,14 +4089,14 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
-      <c r="Z20" s="5" t="s">
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AA20" s="5" t="s">
+      <c r="AC20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
@@ -4002,10 +4184,10 @@
       <c r="O21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="4" t="s">
+      <c r="P21" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="32" t="s">
         <v>33</v>
       </c>
       <c r="R21" s="2" t="s">
@@ -4026,14 +4208,14 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
-      <c r="Z21" s="5" t="s">
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AA21" s="5" t="s">
+      <c r="AC21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="6"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
@@ -4145,14 +4327,14 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
-      <c r="Z22" s="5" t="s">
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AA22" s="5" t="s">
+      <c r="AC22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
       <c r="AD22" s="6"/>
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
@@ -4264,14 +4446,14 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
-      <c r="Z23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA23" s="5" t="s">
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
@@ -4338,10 +4520,10 @@
       <c r="H24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="I24" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="20" t="s">
         <v>2</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -4356,7 +4538,7 @@
       <c r="N24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="29" t="s">
         <v>2</v>
       </c>
       <c r="P24" s="3" t="s">

</xml_diff>

<commit_message>
fixed clue layout some more
</commit_message>
<xml_diff>
--- a/ourClueLayout.xlsx
+++ b/ourClueLayout.xlsx
@@ -44,9 +44,6 @@
     <t>Room</t>
   </si>
   <si>
-    <t>GL</t>
-  </si>
-  <si>
     <t>Walkway</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>Exit room target tests (2)</t>
+  </si>
+  <si>
+    <t>GR</t>
   </si>
 </sst>
 </file>
@@ -214,7 +214,7 @@
       <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +329,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6DC037"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -359,7 +365,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -400,12 +406,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,6 +457,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,6 +542,7 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF6DC037"/>
       <color rgb="FF990099"/>
       <color rgb="FFFF6699"/>
       <color rgb="FF666699"/>
@@ -1799,8 +1809,8 @@
   </sheetPr>
   <dimension ref="A1:IV32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AA19" sqref="AA19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1813,77 +1823,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-      <c r="BB1" s="15"/>
-      <c r="BC1" s="15"/>
-      <c r="BD1" s="15"/>
-      <c r="BE1" s="15"/>
-      <c r="BF1" s="15"/>
-      <c r="BG1" s="15"/>
-      <c r="BH1" s="15"/>
-      <c r="BI1" s="15"/>
-      <c r="BJ1" s="15"/>
-      <c r="BK1" s="15"/>
-      <c r="BL1" s="15"/>
-      <c r="BM1" s="15"/>
-      <c r="BN1" s="15"/>
-      <c r="BO1" s="15"/>
-      <c r="BP1" s="15"/>
-      <c r="BQ1" s="15"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+      <c r="BC1" s="32"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
+      <c r="BI1" s="32"/>
+      <c r="BJ1" s="32"/>
+      <c r="BK1" s="32"/>
+      <c r="BL1" s="32"/>
+      <c r="BM1" s="32"/>
+      <c r="BN1" s="32"/>
+      <c r="BO1" s="32"/>
+      <c r="BP1" s="32"/>
+      <c r="BQ1" s="32"/>
     </row>
     <row r="2" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1901,7 +1911,7 @@
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1931,7 +1941,7 @@
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Q2" s="4" t="s">
@@ -1946,7 +1956,7 @@
       <c r="T2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="U2" s="29" t="s">
         <v>2</v>
       </c>
       <c r="V2" s="5">
@@ -1955,7 +1965,7 @@
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
-      <c r="Z2" s="4"/>
+      <c r="Z2" s="33"/>
       <c r="AA2" s="5" t="s">
         <v>7</v>
       </c>
@@ -2133,9 +2143,9 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -2191,7 +2201,7 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
@@ -2271,10 +2281,10 @@
         <v>3</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>10</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>3</v>
@@ -2297,7 +2307,7 @@
       <c r="T5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V5" s="5">
@@ -2308,11 +2318,11 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AD5" s="6"/>
       <c r="AE5" s="6"/>
@@ -2360,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
@@ -2389,10 +2399,10 @@
       <c r="K6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="22" t="s">
+      <c r="L6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="20" t="s">
         <v>2</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -2427,7 +2437,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
@@ -2542,9 +2552,9 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
-      <c r="Z7" s="28"/>
+      <c r="Z7" s="26"/>
       <c r="AA7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
@@ -2596,7 +2606,7 @@
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2614,7 +2624,7 @@
       <c r="H8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="27" t="s">
         <v>2</v>
       </c>
       <c r="J8" s="3" t="s">
@@ -2641,7 +2651,7 @@
       <c r="Q8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R8" s="20" t="s">
+      <c r="R8" s="18" t="s">
         <v>2</v>
       </c>
       <c r="S8" s="3" t="s">
@@ -2650,7 +2660,7 @@
       <c r="T8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="U8" s="18" t="s">
+      <c r="U8" s="16" t="s">
         <v>2</v>
       </c>
       <c r="V8" s="5">
@@ -2659,9 +2669,9 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
-      <c r="Z8" s="17"/>
+      <c r="Z8" s="15"/>
       <c r="AA8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
@@ -2708,67 +2718,67 @@
     </row>
     <row r="9" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="J9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="K9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="L9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="M9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="N9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="O9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="R9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="S9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="T9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="U9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V9" s="5">
         <v>7</v>
@@ -2776,9 +2786,9 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
-      <c r="Z9" s="19"/>
+      <c r="Z9" s="17"/>
       <c r="AA9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
@@ -2825,67 +2835,67 @@
     </row>
     <row r="10" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="J10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="K10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="L10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="M10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="N10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="O10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="R10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="S10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="T10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="U10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V10" s="5">
         <v>8</v>
@@ -2893,9 +2903,9 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
-      <c r="Z10" s="21"/>
+      <c r="Z10" s="19"/>
       <c r="AA10" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
@@ -2942,67 +2952,67 @@
     </row>
     <row r="11" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="J11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="K11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="L11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="M11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="N11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="8" t="s">
+      <c r="O11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="S11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="T11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="U11" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V11" s="5">
         <v>9</v>
@@ -3010,9 +3020,9 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="21"/>
       <c r="AA11" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
@@ -3059,67 +3069,67 @@
     </row>
     <row r="12" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="J12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="K12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="L12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="M12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="8" t="s">
+      <c r="N12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="S12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="T12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="U12" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V12" s="5">
         <v>10</v>
@@ -3127,13 +3137,13 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
-      <c r="Z12" s="25"/>
+      <c r="Z12" s="23"/>
       <c r="AA12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB12" s="6"/>
       <c r="AC12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AD12" s="6"/>
       <c r="AE12" s="6"/>
@@ -3178,67 +3188,67 @@
     </row>
     <row r="13" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="J13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="K13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="L13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="M13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="8" t="s">
+      <c r="N13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="R13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="S13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="T13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="U13" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V13" s="5">
         <v>11</v>
@@ -3246,15 +3256,15 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
-      <c r="Z13" s="27"/>
+      <c r="Z13" s="25"/>
       <c r="AA13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
@@ -3299,67 +3309,67 @@
     </row>
     <row r="14" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="J14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="K14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="L14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="M14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="N14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="8" t="s">
+      <c r="O14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="R14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="S14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="T14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="U14" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="V14" s="5">
         <v>12</v>
@@ -3367,15 +3377,15 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
-      <c r="Z14" s="29"/>
+      <c r="Z14" s="27"/>
       <c r="AA14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB14" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AD14" s="6"/>
       <c r="AE14" s="6"/>
@@ -3420,49 +3430,49 @@
     </row>
     <row r="15" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="J15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="K15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="L15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="M15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="N15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="O15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>2</v>
@@ -3476,7 +3486,7 @@
       <c r="S15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T15" s="16" t="s">
+      <c r="T15" s="14" t="s">
         <v>2</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -3488,15 +3498,15 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
-      <c r="Z15" s="30"/>
+      <c r="Z15" s="28"/>
       <c r="AA15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AB15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC15" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="AD15" s="6"/>
       <c r="AE15" s="6"/>
@@ -3541,22 +3551,22 @@
     </row>
     <row r="16" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>2</v>
@@ -3588,20 +3598,20 @@
       <c r="P16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="26" t="s">
+      <c r="Q16" s="24" t="s">
         <v>2</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V16" s="5">
         <v>14</v>
@@ -3609,15 +3619,15 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
-      <c r="Z16" s="31"/>
+      <c r="Z16" s="29"/>
       <c r="AA16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AD16" s="6"/>
       <c r="AE16" s="6"/>
@@ -3667,7 +3677,7 @@
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -3685,7 +3695,7 @@
       <c r="H17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="22" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="3" t="s">
@@ -3710,19 +3720,19 @@
         <v>2</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V17" s="5">
         <v>15</v>
@@ -3730,15 +3740,15 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
-      <c r="Z17" s="32"/>
+      <c r="Z17" s="30"/>
       <c r="AA17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AB17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC17" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="AC17" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="AD17" s="6"/>
       <c r="AE17" s="6"/>
@@ -3782,7 +3792,7 @@
       <c r="BQ17" s="6"/>
     </row>
     <row r="18" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="27" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -3813,16 +3823,16 @@
         <v>2</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>2</v>
@@ -3834,16 +3844,16 @@
         <v>2</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V18" s="5">
         <v>16</v>
@@ -3857,7 +3867,7 @@
         <v>5</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AD18" s="6"/>
       <c r="AE18" s="6"/>
@@ -3902,26 +3912,26 @@
     </row>
     <row r="19" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>31</v>
-      </c>
       <c r="H19" s="3" t="s">
         <v>2</v>
       </c>
@@ -3932,16 +3942,16 @@
         <v>2</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>2</v>
@@ -3952,7 +3962,7 @@
       <c r="Q19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R19" s="22" t="s">
+      <c r="R19" s="20" t="s">
         <v>2</v>
       </c>
       <c r="S19" s="3" t="s">
@@ -3961,7 +3971,7 @@
       <c r="T19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="U19" s="29" t="s">
+      <c r="U19" s="27" t="s">
         <v>2</v>
       </c>
       <c r="V19" s="5">
@@ -3973,10 +3983,10 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AD19" s="6"/>
       <c r="AE19" s="6"/>
@@ -4021,25 +4031,25 @@
     </row>
     <row r="20" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>2</v>
@@ -4051,16 +4061,16 @@
         <v>2</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>2</v>
@@ -4069,19 +4079,19 @@
         <v>2</v>
       </c>
       <c r="Q20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="S20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="T20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V20" s="5">
         <v>18</v>
@@ -4092,10 +4102,10 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
       <c r="AB20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AD20" s="6"/>
       <c r="AE20" s="6"/>
@@ -4140,25 +4150,25 @@
     </row>
     <row r="21" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>2</v>
@@ -4170,37 +4180,37 @@
         <v>2</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P21" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q21" s="32" t="s">
-        <v>33</v>
+      <c r="P21" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V21" s="5">
         <v>19</v>
@@ -4211,10 +4221,10 @@
       <c r="Z21" s="5"/>
       <c r="AA21" s="5"/>
       <c r="AB21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AD21" s="6"/>
       <c r="AE21" s="6"/>
@@ -4259,25 +4269,25 @@
     </row>
     <row r="22" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>2</v>
@@ -4289,16 +4299,16 @@
         <v>2</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O22" s="3" t="s">
         <v>2</v>
@@ -4307,19 +4317,19 @@
         <v>2</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V22" s="5">
         <v>20</v>
@@ -4330,10 +4340,10 @@
       <c r="Z22" s="5"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD22" s="6"/>
       <c r="AE22" s="6"/>
@@ -4378,25 +4388,25 @@
     </row>
     <row r="23" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>2</v>
@@ -4408,16 +4418,16 @@
         <v>2</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
+      </c>
+      <c r="N23" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="O23" s="3" t="s">
         <v>2</v>
@@ -4426,19 +4436,19 @@
         <v>2</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V23" s="5">
         <v>21</v>
@@ -4452,7 +4462,7 @@
         <v>2</v>
       </c>
       <c r="AC23" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AD23" s="6"/>
       <c r="AE23" s="6"/>
@@ -4497,67 +4507,67 @@
     </row>
     <row r="24" spans="1:69" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I24" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J24" s="20" t="s">
+      <c r="I24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="18" t="s">
         <v>2</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O24" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" s="27" t="s">
         <v>2</v>
       </c>
       <c r="P24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="V24" s="5">
         <v>22</v>

</xml_diff>